<commit_message>
Debugged - ready to show
</commit_message>
<xml_diff>
--- a/Output/SDTM_Results.xlsx
+++ b/Output/SDTM_Results.xlsx
@@ -2811,7 +2811,11 @@
           <t>TI</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr"/>
+      <c r="C2" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D2" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;have had a diagnosis of either:&lt;/p&gt;\n&lt;ul&gt;\n  &lt;li&gt;\n    &lt;p&gt;[1a] T1DM based on the World Health Organization (WHO) diagnostic criteria, and have been on the following daily insulin therapy for at least 1 year&lt;/p&gt;\n    &lt;ul&gt;\n      &lt;p&gt;[A] multiple daily injection of long-acting insulin analog (either insulin glargine [U-100 or U-300] or insulin degludec [U-100]) and rapid-acting insulin analog (insulin lispro, insulin aspart, or insulin glulisine), or&lt;/p&gt;\n      &lt;p&gt;[B] continuous subcutaneous insulin infusion (CSII)&lt;/p&gt;    \n    &lt;/ul&gt;\n  &lt;/li&gt;\n  &lt;p&gt;Or&lt;/p&gt;\n  &lt;li&gt;\n    &lt;p&gt;[1b] T2DM based on the WHO diagnostic criteria, and have received the&lt;/p&gt;\n    &lt;p&gt;following daily insulin therapy with or without oral anti-hyperglycemic medications (OAMs) for at least 1 year&lt;/p&gt;\n    &lt;ul&gt;\n      &lt;p&gt;[A] insulin: long-acting insulin analog (either insulin glargine [U-100 or U-300] or insulin degludec [U-100]) alone, or in combination with rapid-acting insulin analog (insulin lispro, insulin aspart, or insulin glulisine) or CSII&lt;/p&gt;\n      &lt;p&gt;[B] OAM: up to 3 of the following OAMs in accordance with local regulations: metformin, dipeptidyl peptidase-4 inhibitor, sodium glucose cotransporter 2 inhibitor, sulfonylurea (should not be more than half of maximum approved doses), glinides, alpha-glucosidase inhibitor, or thiazolidine&lt;/p&gt;\n    &lt;/ul&gt;\n  &lt;/li&gt;\n&lt;/ul&gt;</t>
@@ -2841,15 +2845,19 @@
     <row r="3" ht="29" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>DOMAIN</t>
+          <t> </t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Domain Abbreviation</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;male patients: agree to use an effective method of contraception for the duration of the study and for 28 days following the last study treatment&lt;/p&gt;</t>
@@ -2872,22 +2880,26 @@
       </c>
       <c r="H3" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4" ht="29" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>IETESTCD</t>
+          <t> </t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Incl/Excl Criterion Short Name</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D4" s="9" t="inlineStr">
         <is>
           <t>&lt;ul&gt;\n  &lt;li&gt;\n    [3a] women of childbearing potential who are abstinent (if this is complete\n    abstinence, as their preferred and usual lifestyle) or in a same sex\n    relationship (as part of their preferred and usual lifestyle) must agree to\n    either remain abstinent or stay in a same sex relationship without sexual\n    relationships with males. Periodic abstinence (eg, calendar, ovulation,\n    symptothermal, post-ovulation methods), declaration of abstinence just for\n    the duration of a trial, and withdrawal are not acceptable methods of\n    contraception.\n  &lt;/li&gt;\n  &lt;li&gt;\n    [3b] otherwise, women of childbearing potential participating must agree to use\n    one highly effective method (less than 1% failure rate) of contraception, or a\n    combination of 2 effective methods of contraception for the entirety of the\n    study.\n    &lt;ul&gt;\n      &lt;li&gt;[A] women of childbearing potential participating must test negative for\n        pregnancy prior to initiation of treatment as indicated by a negative serum\n        pregnancy test at the screening visit followed by a negative urine\n        pregnancy test within 24 hours prior to exposure.&lt;/li&gt;\n      &lt;li&gt;[B] either one highly effective method of contraception or a combination\n        of 2 effective methods of contraception will be used. The patient may\n        choose to use a double barrier method of contraception. Barrier protection\n        methods without concomitant use of a spermicide are not a reliable or\n        acceptable method. Thus, each barrier method must include use of a\n        spermicide. It should be noted that the use of male and female condoms\n        as a double barrier method is not considered acceptable due to the high\n        failure rate when these methods are combined.&lt;/li&gt;\n    &lt;/ul&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    [3c] women not of childbearing potential may participate, and include those who are:\n    &lt;ul&gt;\n      &lt;li&gt;\n        [A] infertile due to surgical sterilization (hysterectomy, bilateral\n        oophorectomy, or tubal ligation), congenital anomaly such as mullerian\n        agenesis\n      &lt;/li&gt;\n      &lt;li&gt;\n        Or\n        [B] postmenopausal, defined as either:\n        &lt;ul&gt;\n          &lt;li&gt;[i] a woman at least 50 years of age with an intact uterus, not on hormone therapy, who has had either:\n          &lt;/li&gt;\n          &lt;ul&gt;\n            &lt;li&gt;[a] cessation of menses for at least 1 year, or&lt;/li&gt;\n            &lt;li&gt;[b] at least 6 months of spontaneous amenorrhea with a follicle-stimulating hormone &gt;40 mIU/mL; or&lt;/li&gt;\n          &lt;/ul&gt;\n          &lt;li&gt;[ii] a woman 55 or older not on hormone therapy, who has had at least 6 months of spontaneous amenorrhea,\n            or&lt;/li&gt;\n          &lt;li&gt;[iii] a woman at least 55 years of age with a diagnosis of menopause prior to starting hormone replacement\n            therapy&lt;/li&gt;\n        &lt;/ul&gt;\n      &lt;/li&gt;\n    &lt;/ul&gt;\n  &lt;/li&gt;\n&lt;/ul&gt;</t>
@@ -2908,20 +2920,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H4" s="33" t="n"/>
+      <c r="H4" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="87" customHeight="1">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>IETEST</t>
+          <t> </t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>Inclusion/Exclusion Criterion</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;are between 18 and 64 years old for T1DM, or between 20 and 70 years old for T2DM at the time of informed consent&lt;/p&gt;</t>
@@ -2942,20 +2962,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H5" s="33" t="n"/>
+      <c r="H5" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>IECAT</t>
+          <t> </t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>Inclusion/Exclusion Category</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;have a body mass index of 18.5 to 30.0 kg/m 2 for T1DM, or 18.5 to 35.0 kg/m 2 for T2DM at the time of screening&lt;/p&gt;</t>
@@ -2976,20 +3004,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H6" s="33" t="n"/>
+      <c r="H6" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="43.5" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>IESCAT</t>
+          <t> </t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>Inclusion/Exclusion Subcategory</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;have a hemoglobin A1c value ≤10% at the time of screening&lt;/p&gt;</t>
@@ -3010,20 +3046,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H7" s="33" t="n"/>
+      <c r="H7" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="29" customHeight="1">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>TIRL</t>
+          <t> </t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>Inclusion/Exclusion Criterion Rule</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;have clinical laboratory test results within normal reference range (except for glycemic parameters) for the population or investigative site, or results with acceptable deviations that are judged to be not clinically significant by the investigator&lt;/p&gt;</t>
@@ -3044,20 +3088,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H8" s="33" t="n"/>
+      <c r="H8" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>TIVERS</t>
+          <t> </t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>Protocol Criteria Versions</t>
-        </is>
-      </c>
-      <c r="C9" s="9" t="inlineStr"/>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="D9" s="9" t="inlineStr">
         <is>
           <t>&lt;p&gt;have venous access sufficient to allow for blood sampling and administration of insulin for IV administration as per the protocol&lt;/p&gt;</t>
@@ -3078,10 +3130,28 @@
           <t> </t>
         </is>
       </c>
-      <c r="H9" s="33" t="n"/>
+      <c r="H9" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>&lt;p&gt;are reliable and willing to make themselves available for the duration of the study and are willing to follow study procedures&lt;/p&gt;</t>
@@ -3102,8 +3172,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>10</t>
@@ -3129,8 +3214,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>11</t>
@@ -3156,8 +3256,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>12</t>
@@ -3183,8 +3298,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>13</t>
@@ -3210,8 +3340,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>14</t>
@@ -3237,8 +3382,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>15</t>
@@ -3264,8 +3424,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>16</t>
@@ -3291,8 +3466,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>17</t>
@@ -3318,8 +3508,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>18</t>
@@ -3345,8 +3550,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>19</t>
@@ -3372,8 +3592,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>20</t>
@@ -3399,8 +3634,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>21</t>
@@ -3426,8 +3676,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>22</t>
@@ -3453,8 +3718,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>23</t>
@@ -3480,8 +3760,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>24</t>
@@ -3507,8 +3802,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>25</t>
@@ -3534,8 +3844,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>26</t>
@@ -3561,8 +3886,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>27</t>
@@ -3588,8 +3928,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>28</t>
@@ -3615,8 +3970,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>29</t>
@@ -3642,8 +4012,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>30</t>
@@ -3669,8 +4054,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>31</t>
@@ -3696,8 +4096,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>32</t>
@@ -3723,8 +4138,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>33</t>
@@ -3750,8 +4180,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>34</t>
@@ -3777,8 +4222,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>35</t>
@@ -3804,8 +4264,23 @@
           <t> </t>
         </is>
       </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>36</t>
@@ -3829,6 +4304,11 @@
       <c r="G37" t="inlineStr">
         <is>
           <t> </t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
create TE and a bug fix
</commit_message>
<xml_diff>
--- a/Output/SDTM_Results.xlsx
+++ b/Output/SDTM_Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-10890" yWindow="-20340" windowWidth="31995" windowHeight="17895" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-4515" yWindow="-19065" windowWidth="27645" windowHeight="13335" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" state="visible" r:id="rId1"/>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -141,6 +141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.7999816888943144"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +284,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -341,17 +347,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -397,9 +394,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -418,11 +412,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -850,101 +859,69 @@
       </c>
       <c r="B7" s="17" t="n"/>
     </row>
-    <row r="9" ht="31" customHeight="1">
+    <row r="9" ht="15.5" customHeight="1">
       <c r="A9" s="18" t="inlineStr">
         <is>
-          <t>Class</t>
+          <t>Mapping Name</t>
         </is>
       </c>
       <c r="B9" s="18" t="inlineStr">
         <is>
-          <t>The target class in USDM where the M11 element is mapped</t>
+          <t>The name of the original mapping in DDF USDM v4.0</t>
         </is>
       </c>
     </row>
     <row r="10" ht="31" customHeight="1">
       <c r="A10" s="18" t="inlineStr">
         <is>
-          <t>Attribute</t>
+          <t>JSONATA</t>
         </is>
       </c>
       <c r="B10" s="18" t="inlineStr">
         <is>
-          <t>The target attribute in USDM where the M11 element is mapped</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="15.5" customHeight="1">
+          <t>The USDM v4.0 mappings combined to a JSONATA query</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="31" customHeight="1">
       <c r="A11" s="18" t="inlineStr">
         <is>
-          <t>Overall Notes</t>
+          <t>Fixed Content</t>
         </is>
       </c>
       <c r="B11" s="18" t="inlineStr">
         <is>
-          <t>Notes on the overall mapping</t>
+          <t>In case content is fixed and no mapping is needed the corresponding value is presented in this column</t>
         </is>
       </c>
     </row>
     <row r="12" ht="31" customHeight="1">
       <c r="A12" s="18" t="inlineStr">
         <is>
-          <t>Target Path</t>
+          <t>TSVALNF (in case of TS)</t>
         </is>
       </c>
       <c r="B12" s="18" t="inlineStr">
         <is>
-          <t>The full path to the place in USDM holding the dtaa for the M11 element</t>
+          <t>value to be presented in case no value is returned based on a JSONATA query</t>
         </is>
       </c>
     </row>
     <row r="13" ht="15.5" customHeight="1">
-      <c r="A13" s="18" t="inlineStr">
-        <is>
-          <t>Target Notes</t>
-        </is>
-      </c>
-      <c r="B13" s="18" t="inlineStr">
-        <is>
-          <t>Any notes relating to the target path</t>
-        </is>
-      </c>
+      <c r="A13" s="18" t="n"/>
+      <c r="B13" s="18" t="n"/>
     </row>
     <row r="14" ht="15.5" customHeight="1">
-      <c r="A14" s="18" t="inlineStr">
-        <is>
-          <t>Condition Path</t>
-        </is>
-      </c>
-      <c r="B14" s="18" t="inlineStr">
-        <is>
-          <t>The conditions applicable to the target path mapping</t>
-        </is>
-      </c>
+      <c r="A14" s="18" t="n"/>
+      <c r="B14" s="18" t="n"/>
     </row>
     <row r="15" ht="15.5" customHeight="1">
-      <c r="A15" s="18" t="inlineStr">
-        <is>
-          <t>Condition Notes</t>
-        </is>
-      </c>
-      <c r="B15" s="18" t="inlineStr">
-        <is>
-          <t>Any associated notes relevant to the conditions</t>
-        </is>
-      </c>
+      <c r="A15" s="18" t="n"/>
+      <c r="B15" s="18" t="n"/>
     </row>
     <row r="16" ht="15.5" customHeight="1">
-      <c r="A16" s="18" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="B16" s="18" t="inlineStr">
-        <is>
-          <t>Mapping status, either "Mapped" or "To Be Mapped"</t>
-        </is>
-      </c>
+      <c r="A16" s="18" t="n"/>
+      <c r="B16" s="18" t="n"/>
     </row>
     <row r="18" ht="21" customHeight="1">
       <c r="A18" s="17" t="inlineStr">
@@ -954,27 +931,27 @@
       </c>
       <c r="B18" s="17" t="n"/>
     </row>
-    <row r="20" ht="77.5" customHeight="1">
+    <row r="20" ht="62" customHeight="1">
       <c r="A20" s="18" t="inlineStr">
         <is>
-          <t>Class and Attribute</t>
+          <t>Multiple Mappings</t>
         </is>
       </c>
       <c r="B20" s="18" t="inlineStr">
         <is>
-          <t>The specified class and attribute to be used in a mapping are specified up to the level of reference, the complex datatype or lower if needed for specificity. The corresponding path further specifies specific the exact attributes used from complex datatypes or subclasses.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="77.5" customHeight="1">
-      <c r="A21" s="18" t="inlineStr">
-        <is>
-          <t>Multiple Mappings</t>
-        </is>
-      </c>
-      <c r="B21" s="18" t="inlineStr">
-        <is>
-          <t>In some cases there is more than one mapping for the same M11 item. These mappings are usually distinct where either one of them may be used (and the other is expected to be not available) or they need to be all combined for the M11 item.</t>
+          <t xml:space="preserve">In case there is more than one mapping for the same SDTM item these mappings are provided in separate rows in the USDM v4.0 mapping file. In this mapping file, they are combined again to 1 JSONata query. </t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="43.5" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Resulting domains</t>
+        </is>
+      </c>
+      <c r="B21" s="46" t="inlineStr">
+        <is>
+          <t>For the resulting domains, the specified variables are transposed to columns and the result values are presented in rows.</t>
         </is>
       </c>
     </row>
@@ -991,15 +968,15 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col width="17.81640625" customWidth="1" min="1" max="2"/>
     <col width="25.81640625" customWidth="1" min="6" max="6"/>
-    <col width="30.08984375" customWidth="1" style="41" min="7" max="7"/>
+    <col width="30.08984375" customWidth="1" style="46" min="7" max="7"/>
     <col width="18.6328125" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -1034,19 +1011,19 @@
           <t>Mapping Name</t>
         </is>
       </c>
-      <c r="G1" s="37" t="inlineStr">
+      <c r="G1" s="34" t="inlineStr">
         <is>
           <t>JSONATA</t>
         </is>
       </c>
-      <c r="H1" s="27" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>Fixed content</t>
         </is>
       </c>
-      <c r="I1" s="27" t="n"/>
-      <c r="J1" s="27" t="n"/>
-      <c r="K1" s="27" t="n"/>
+      <c r="I1" s="24" t="n"/>
+      <c r="J1" s="24" t="n"/>
+      <c r="K1" s="24" t="n"/>
     </row>
     <row r="2" ht="72.5" customHeight="1">
       <c r="A2" s="7" t="inlineStr">
@@ -1084,7 +1061,7 @@
           <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
         </is>
       </c>
-      <c r="H2" s="33" t="n"/>
+      <c r="H2" s="30" t="n"/>
       <c r="I2" s="16" t="n"/>
       <c r="J2" s="16" t="n"/>
       <c r="K2" s="16" t="n"/>
@@ -1417,10 +1394,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
@@ -1428,448 +1405,289 @@
     <col width="18.36328125" customWidth="1" min="1" max="1"/>
     <col width="20.36328125" customWidth="1" min="2" max="2"/>
     <col width="9.36328125" customWidth="1" min="3" max="5"/>
-    <col width="18.1796875" customWidth="1" min="6" max="6"/>
-    <col width="18.81640625" customWidth="1" min="7" max="7"/>
-    <col width="39.453125" customWidth="1" min="8" max="9"/>
-    <col width="25.81640625" customWidth="1" min="10" max="10"/>
-    <col width="49.36328125" customWidth="1" min="11" max="11"/>
-    <col width="45.6328125" customWidth="1" min="12" max="12"/>
-    <col width="25.81640625" customWidth="1" min="13" max="13"/>
-    <col width="15.36328125" customWidth="1" style="23" min="16" max="16"/>
+    <col width="25.81640625" customWidth="1" min="6" max="6"/>
+    <col width="39.90625" customWidth="1" min="7" max="7"/>
+    <col width="10.81640625" customWidth="1" style="46" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" s="49" t="inlineStr">
-        <is>
-          <t>SDTM</t>
-        </is>
-      </c>
-      <c r="B1" s="50" t="n"/>
-      <c r="C1" s="50" t="n"/>
-      <c r="D1" s="50" t="n"/>
-      <c r="E1" s="51" t="n"/>
-      <c r="F1" s="42" t="inlineStr">
-        <is>
-          <t>USDM</t>
-        </is>
-      </c>
-      <c r="G1" s="50" t="n"/>
-      <c r="H1" s="50" t="n"/>
-      <c r="I1" s="50" t="n"/>
-      <c r="J1" s="50" t="n"/>
-      <c r="K1" s="50" t="n"/>
-      <c r="L1" s="50" t="n"/>
-      <c r="M1" s="50" t="n"/>
-      <c r="N1" s="50" t="n"/>
-      <c r="O1" s="50" t="n"/>
-      <c r="P1" s="51" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Variable Name </t>
-        </is>
-      </c>
-      <c r="B2" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Variable Label </t>
-        </is>
-      </c>
-      <c r="C2" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Type </t>
-        </is>
-      </c>
-      <c r="D2" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Role </t>
-        </is>
-      </c>
-      <c r="E2" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Core </t>
-        </is>
-      </c>
-      <c r="F2" s="11" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
-      </c>
-      <c r="G2" s="11" t="inlineStr">
-        <is>
-          <t>Attribute</t>
-        </is>
-      </c>
-      <c r="H2" s="11" t="inlineStr">
-        <is>
-          <t>Overall Notes</t>
-        </is>
-      </c>
-      <c r="I2" s="11" t="inlineStr">
-        <is>
-          <t>Target Path</t>
-        </is>
-      </c>
-      <c r="J2" s="11" t="inlineStr">
-        <is>
-          <t>Target Notes</t>
-        </is>
-      </c>
-      <c r="K2" s="11" t="inlineStr">
-        <is>
-          <t>Condition Path</t>
-        </is>
-      </c>
-      <c r="L2" s="11" t="inlineStr">
-        <is>
-          <t>Condition Notes</t>
-        </is>
-      </c>
-      <c r="M2" s="11" t="inlineStr">
-        <is>
-          <t>Mapping Name</t>
-        </is>
-      </c>
-      <c r="N2" s="11" t="inlineStr">
-        <is>
-          <t>Mapping Category</t>
-        </is>
-      </c>
-      <c r="O2" s="11" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="P2" s="24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">v4.0 Change </t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="77.5" customHeight="1">
+    <row r="1" ht="42" customHeight="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>STUDYID</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>DOMAIN</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>ETCD</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>ELEMENT</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>TESTRL</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>TEENRL</t>
+        </is>
+      </c>
+      <c r="G1" s="34" t="inlineStr">
+        <is>
+          <t>TEDUR</t>
+        </is>
+      </c>
+      <c r="H1" s="45" t="inlineStr">
+        <is>
+          <t>Fixed content</t>
+        </is>
+      </c>
+      <c r="I1" s="24" t="n"/>
+      <c r="J1" s="24" t="n"/>
+      <c r="K1" s="24" t="n"/>
+    </row>
+    <row r="2" ht="58" customHeight="1">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>I8R-JE-IGBJ</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr"/>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>Screening Element</t>
+        </is>
+      </c>
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>Study Start</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t>Day -1 of treatment period 1</t>
+        </is>
+      </c>
+      <c r="G2" s="31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H2" s="48" t="n"/>
+      <c r="I2" s="16" t="n"/>
+      <c r="J2" s="16" t="n"/>
+      <c r="K2" s="16" t="n"/>
+    </row>
+    <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>STUDYID</t>
+          <t>I8R-JE-IGBJ</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Study Identifier</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr"/>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>IM Glucagon + LY900018</t>
         </is>
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F3" s="6" t="inlineStr">
-        <is>
-          <t>StudyIdentifier</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="8" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyIdentifiers/StudyIdentifier/@text</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="n"/>
-      <c r="K3" s="8" t="inlineStr">
-        <is>
-          <t>StudyRole/@code/Code/@code="C70793" | 
-StudyRole/@organizations | 
-StudyVersion/@studyIdentifiers/StudyIdentifier/@scope</t>
-        </is>
-      </c>
-      <c r="L3" s="8" t="inlineStr">
-        <is>
-          <t>Identifies the sponsor role | 
-Identifies the sponsor organization from the role | 
-Identifies the sponsor organization from the study identifier</t>
-        </is>
-      </c>
-      <c r="M3" s="8" t="inlineStr">
-        <is>
-          <t>Sponsor Study Identifier</t>
-        </is>
-      </c>
-      <c r="N3" s="8" t="inlineStr">
-        <is>
-          <t>Study Identifier</t>
-        </is>
-      </c>
-      <c r="O3" s="8" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P3" s="22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Y </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+          <t>Day -1 of treatment period</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>End of Day 1 of treatment period</t>
+        </is>
+      </c>
+      <c r="G3" s="35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="I3" s="16" t="n"/>
+      <c r="J3" s="16" t="n"/>
+      <c r="K3" s="16" t="n"/>
+    </row>
+    <row r="4" ht="29" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>DOMAIN</t>
+          <t>I8R-JE-IGBJ</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Domain Abbreviation</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr"/>
       <c r="D4" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>Wash Out Element</t>
         </is>
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="9" t="inlineStr">
-        <is>
-          <t>Set to "TA"</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="4" t="n"/>
-      <c r="K4" s="5" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="4" t="n"/>
-      <c r="O4" s="4" t="n"/>
-      <c r="P4" s="25" t="n"/>
+          <t>End of Day 1 of Treatment period 1</t>
+        </is>
+      </c>
+      <c r="F4" s="12" t="inlineStr">
+        <is>
+          <t>Day -1 of treatment period 2</t>
+        </is>
+      </c>
+      <c r="G4" s="47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="29" customHeight="1">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>ETCD</t>
+          <t>I8R-JE-IGBJ</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>Element Code</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr"/>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>Topic</t>
+          <t>IM Glucagon</t>
         </is>
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
+          <t>Day -1 of treatment period</t>
         </is>
       </c>
       <c r="F5" s="12" t="inlineStr">
         <is>
-          <t>StudyElement</t>
-        </is>
-      </c>
-      <c r="G5" s="12" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="H5" s="4" t="n"/>
-      <c r="I5" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label</t>
-        </is>
-      </c>
-      <c r="J5" s="4" t="inlineStr"/>
-      <c r="K5" s="9" t="inlineStr"/>
-      <c r="L5" s="9" t="inlineStr"/>
-      <c r="M5" s="12" t="inlineStr">
-        <is>
-          <t>Element Name</t>
-        </is>
-      </c>
-      <c r="N5" s="4" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O5" s="4" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P5" s="25" t="n"/>
+          <t>End of Day 1 of treatment period</t>
+        </is>
+      </c>
+      <c r="G5" s="47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="29" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>ELEMENT</t>
+          <t>I8R-JE-IGBJ</t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>Description of Element</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr"/>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>Follow Up Element</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>End of Day 1 of Treatment period 2</t>
+        </is>
+      </c>
+      <c r="F6" s="12" t="inlineStr">
+        <is>
+          <t>Leave Study</t>
+        </is>
+      </c>
+      <c r="G6" s="47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="29" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>TEENRL</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>Rule for End of Element</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
         <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>Synonym Qualifier</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F6" s="12" t="inlineStr">
-        <is>
-          <t>StudyElement</t>
-        </is>
-      </c>
-      <c r="G6" s="12" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="n"/>
-      <c r="I6" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@description</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr"/>
-      <c r="K6" s="9" t="inlineStr"/>
-      <c r="L6" s="9" t="inlineStr"/>
-      <c r="M6" s="12" t="inlineStr">
-        <is>
-          <t>Element Description</t>
-        </is>
-      </c>
-      <c r="N6" s="4" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O6" s="4" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P6" s="25" t="n"/>
-    </row>
-    <row r="7" ht="43.5" customHeight="1">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>TESTRL</t>
-        </is>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>Rule for Start of Element</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>Rule</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>Perm</t>
+        </is>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>Element End Rule</t>
+        </is>
+      </c>
+      <c r="G7" s="47" t="inlineStr">
+        <is>
+          <t>study.versions.studyDesigns.elements.{id: transitionEndRule.text}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="29" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>TEDUR</t>
+        </is>
+      </c>
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Planned Duration of Element</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
         <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Rule</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F7" s="12" t="inlineStr">
-        <is>
-          <t>TransitionRule</t>
-        </is>
-      </c>
-      <c r="G7" s="12" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="n"/>
-      <c r="I7" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@transitionStartRule/TransitionRule/@text</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr"/>
-      <c r="K7" s="9" t="inlineStr"/>
-      <c r="L7" s="9" t="inlineStr"/>
-      <c r="M7" s="12" t="inlineStr">
-        <is>
-          <t>Element Start Rule</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P7" s="25" t="n"/>
-    </row>
-    <row r="8" ht="43.5" customHeight="1">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>TEENRL</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="inlineStr">
-        <is>
-          <t>Rule for End of Element</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t>Rule</t>
+          <t>Timing</t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
@@ -1879,123 +1697,11 @@
       </c>
       <c r="F8" s="12" t="inlineStr">
         <is>
-          <t>TransitionRule</t>
-        </is>
-      </c>
-      <c r="G8" s="12" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@transitionEndRule/TransitionRule/@text</t>
-        </is>
-      </c>
-      <c r="J8" s="4" t="inlineStr"/>
-      <c r="K8" s="9" t="inlineStr"/>
-      <c r="L8" s="9" t="inlineStr"/>
-      <c r="M8" s="12" t="inlineStr">
-        <is>
-          <t>Element End Rule</t>
-        </is>
-      </c>
-      <c r="N8" s="4" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O8" s="4" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P8" s="25" t="n"/>
-    </row>
-    <row r="9" ht="145" customHeight="1">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>TEDUR</t>
-        </is>
-      </c>
-      <c r="B9" s="9" t="inlineStr">
-        <is>
-          <t>Planned Duration of Element</t>
-        </is>
-      </c>
-      <c r="C9" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Timing</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="F9" s="12" t="inlineStr">
-        <is>
-          <t>Timing</t>
-        </is>
-      </c>
-      <c r="G9" s="12" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@timings/Timing/@value</t>
-        </is>
-      </c>
-      <c r="J9" s="12" t="inlineStr">
-        <is>
-          <t>The element length can be calculated based on timing values based on the used logic for a trial. For example select the last timing value of epoch related to the element and subtract the timing value of the last scheduledInstance referencing to the previous epoch.</t>
-        </is>
-      </c>
-      <c r="K9" s="12" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements | StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@epoch = StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@instances/ScheduledActivityInstance/@epoch</t>
-        </is>
-      </c>
-      <c r="L9" s="12" t="inlineStr"/>
-      <c r="M9" s="12" t="inlineStr">
-        <is>
           <t>Element Duration</t>
         </is>
       </c>
-      <c r="N9" s="4" t="inlineStr">
-        <is>
-          <t>Study Timeline</t>
-        </is>
-      </c>
-      <c r="O9" s="4" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P9" s="25" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:P1"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K9" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2021,7 +1727,7 @@
     <col width="60.453125" customWidth="1" min="8" max="8"/>
     <col width="26" customWidth="1" min="9" max="13"/>
     <col width="19.453125" customWidth="1" min="14" max="15"/>
-    <col width="16.36328125" customWidth="1" style="23" min="16" max="16"/>
+    <col width="16.36328125" customWidth="1" style="22" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1">
@@ -2034,7 +1740,7 @@
       <c r="C1" s="50" t="n"/>
       <c r="D1" s="50" t="n"/>
       <c r="E1" s="51" t="n"/>
-      <c r="F1" s="42" t="inlineStr">
+      <c r="F1" s="52" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -2204,7 +1910,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P3" s="26" t="inlineStr">
+      <c r="P3" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2250,7 +1956,7 @@
       <c r="M4" s="6" t="n"/>
       <c r="N4" s="6" t="n"/>
       <c r="O4" s="6" t="n"/>
-      <c r="P4" s="26" t="n"/>
+      <c r="P4" s="23" t="n"/>
     </row>
     <row r="5" ht="101.5" customHeight="1">
       <c r="A5" s="6" t="inlineStr">
@@ -2316,7 +2022,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P5" s="26" t="inlineStr">
+      <c r="P5" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2382,7 +2088,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P6" s="26" t="inlineStr">
+      <c r="P6" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2448,7 +2154,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P7" s="26" t="inlineStr">
+      <c r="P7" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2514,7 +2220,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P8" s="26" t="inlineStr">
+      <c r="P8" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2580,7 +2286,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P9" s="26" t="inlineStr">
+      <c r="P9" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2646,7 +2352,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P10" s="26" t="inlineStr">
+      <c r="P10" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2712,7 +2418,7 @@
           <t>Mapped</t>
         </is>
       </c>
-      <c r="P11" s="26" t="inlineStr">
+      <c r="P11" s="23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2742,15 +2448,15 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="G1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col width="18.6328125" customWidth="1" min="1" max="5"/>
     <col width="28.7265625" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="26.6328125" customWidth="1" style="40" min="7" max="7"/>
+    <col width="26.6328125" customWidth="1" style="37" min="7" max="7"/>
     <col width="29.81640625" customWidth="1" style="16" min="8" max="8"/>
     <col width="8.6328125" customWidth="1" style="16" min="9" max="11"/>
   </cols>
@@ -2786,19 +2492,19 @@
           <t>IESCAT</t>
         </is>
       </c>
-      <c r="G1" s="37" t="inlineStr">
+      <c r="G1" s="34" t="inlineStr">
         <is>
           <t>TIRL</t>
         </is>
       </c>
-      <c r="H1" s="27" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>TIVERS</t>
         </is>
       </c>
-      <c r="I1" s="27" t="n"/>
-      <c r="J1" s="27" t="n"/>
-      <c r="K1" s="27" t="n"/>
+      <c r="I1" s="24" t="n"/>
+      <c r="J1" s="24" t="n"/>
+      <c r="K1" s="24" t="n"/>
     </row>
     <row r="2" ht="72.5" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
@@ -2831,12 +2537,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G2" s="34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H2" s="33" t="inlineStr">
+      <c r="G2" s="31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H2" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2873,7 +2579,7 @@
           <t> </t>
         </is>
       </c>
-      <c r="G3" s="38" t="inlineStr">
+      <c r="G3" s="35" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -2915,12 +2621,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G4" s="39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="G4" s="48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2957,12 +2663,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G5" s="41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H5" s="33" t="inlineStr">
+      <c r="G5" s="46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H5" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2999,12 +2705,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G6" s="39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H6" s="33" t="inlineStr">
+      <c r="G6" s="48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H6" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3041,12 +2747,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G7" s="39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H7" s="33" t="inlineStr">
+      <c r="G7" s="48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H7" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3083,12 +2789,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G8" s="38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H8" s="33" t="inlineStr">
+      <c r="G8" s="35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H8" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3125,12 +2831,12 @@
           <t> </t>
         </is>
       </c>
-      <c r="G9" s="38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H9" s="33" t="inlineStr">
+      <c r="G9" s="35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H9" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4325,8 +4031,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -4377,22 +4083,22 @@
           <t>TSVAL</t>
         </is>
       </c>
-      <c r="H1" s="27" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>TSVALNF</t>
         </is>
       </c>
-      <c r="I1" s="27" t="inlineStr">
+      <c r="I1" s="24" t="inlineStr">
         <is>
           <t>TSVALCD</t>
         </is>
       </c>
-      <c r="J1" s="27" t="inlineStr">
+      <c r="J1" s="24" t="inlineStr">
         <is>
           <t>TSVCDREF</t>
         </is>
       </c>
-      <c r="K1" s="27" t="inlineStr">
+      <c r="K1" s="24" t="inlineStr">
         <is>
           <t>TSVCDVER</t>
         </is>
@@ -4429,12 +4135,12 @@
           <t>Planned Minimum Age of Subjects</t>
         </is>
       </c>
-      <c r="G2" s="34" t="inlineStr">
+      <c r="G2" s="31" t="inlineStr">
         <is>
           <t>18  Year</t>
         </is>
       </c>
-      <c r="H2" s="33" t="inlineStr">
+      <c r="H2" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4471,7 +4177,7 @@
           <t>Planned Minimum Age of Subjects</t>
         </is>
       </c>
-      <c r="G3" s="32" t="inlineStr">
+      <c r="G3" s="29" t="inlineStr">
         <is>
           <t>70  Year</t>
         </is>
@@ -4511,12 +4217,12 @@
           <t>Confirmed Response Minimum Duration</t>
         </is>
       </c>
-      <c r="G4" s="32" t="inlineStr">
+      <c r="G4" s="29" t="inlineStr">
         <is>
           <t>1 Day</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4551,12 +4257,12 @@
           <t>Confirmed Response Minimum Duration</t>
         </is>
       </c>
-      <c r="G5" s="32" t="inlineStr">
+      <c r="G5" s="29" t="inlineStr">
         <is>
           <t>1 Day</t>
         </is>
       </c>
-      <c r="H5" s="33" t="inlineStr">
+      <c r="H5" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4591,12 +4297,12 @@
           <t>Dose Level; Dose per Administration</t>
         </is>
       </c>
-      <c r="G6" s="32" t="inlineStr">
+      <c r="G6" s="29" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="H6" s="33" t="inlineStr">
+      <c r="H6" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4631,12 +4337,12 @@
           <t>Dose Level; Dose per Administration</t>
         </is>
       </c>
-      <c r="G7" s="32" t="inlineStr">
+      <c r="G7" s="29" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H7" s="33" t="inlineStr">
+      <c r="H7" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4671,12 +4377,12 @@
           <t>Dosing Frequency</t>
         </is>
       </c>
-      <c r="G8" s="32" t="inlineStr">
+      <c r="G8" s="29" t="inlineStr">
         <is>
           <t>Once</t>
         </is>
       </c>
-      <c r="H8" s="33" t="inlineStr">
+      <c r="H8" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4726,12 +4432,12 @@
           <t>Dosing Frequency</t>
         </is>
       </c>
-      <c r="G9" s="32" t="inlineStr">
+      <c r="G9" s="29" t="inlineStr">
         <is>
           <t>Once</t>
         </is>
       </c>
-      <c r="H9" s="33" t="inlineStr">
+      <c r="H9" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4781,12 +4487,12 @@
           <t>Dose Units</t>
         </is>
       </c>
-      <c r="G10" s="32" t="inlineStr">
+      <c r="G10" s="29" t="inlineStr">
         <is>
           <t>Milligram</t>
         </is>
       </c>
-      <c r="H10" s="33" t="inlineStr">
+      <c r="H10" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4836,12 +4542,12 @@
           <t>Dose Units</t>
         </is>
       </c>
-      <c r="G11" s="32" t="inlineStr">
+      <c r="G11" s="29" t="inlineStr">
         <is>
           <t>Milligram</t>
         </is>
       </c>
-      <c r="H11" s="33" t="inlineStr">
+      <c r="H11" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4891,12 +4597,12 @@
           <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
         </is>
       </c>
-      <c r="G12" s="32" t="inlineStr">
+      <c r="G12" s="29" t="inlineStr">
         <is>
           <t>T1DM</t>
         </is>
       </c>
-      <c r="H12" s="33" t="inlineStr">
+      <c r="H12" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6151,8 +5857,8 @@
   </sheetPr>
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="I1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
@@ -6196,32 +5902,32 @@
           <t>TSGRPID</t>
         </is>
       </c>
-      <c r="F1" s="27" t="inlineStr">
+      <c r="F1" s="24" t="inlineStr">
         <is>
           <t>Mapping Name</t>
         </is>
       </c>
-      <c r="G1" s="27" t="inlineStr">
+      <c r="G1" s="24" t="inlineStr">
         <is>
           <t>Mapping Results</t>
         </is>
       </c>
-      <c r="H1" s="27" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>TSVALNF if empty</t>
         </is>
       </c>
-      <c r="I1" s="27" t="inlineStr">
+      <c r="I1" s="24" t="inlineStr">
         <is>
           <t>TSVALCD JSONATA map</t>
         </is>
       </c>
-      <c r="J1" s="27" t="inlineStr">
+      <c r="J1" s="24" t="inlineStr">
         <is>
           <t>TSVALCDREF JSONATA map</t>
         </is>
       </c>
-      <c r="K1" s="27" t="inlineStr">
+      <c r="K1" s="24" t="inlineStr">
         <is>
           <t>TSVALCDVER JSONATA map</t>
         </is>
@@ -6250,7 +5956,7 @@
           <t>Adaptive Design Indicator</t>
         </is>
       </c>
-      <c r="G2" s="30" t="inlineStr">
+      <c r="G2" s="27" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6294,7 +6000,7 @@
           <t>Study Minimum Age + Unit Study Population</t>
         </is>
       </c>
-      <c r="G3" s="28" t="inlineStr">
+      <c r="G3" s="25" t="inlineStr">
         <is>
           <t>18  Year</t>
         </is>
@@ -6343,12 +6049,12 @@
           <t>Study Maximum Age + Unit Study Population</t>
         </is>
       </c>
-      <c r="G4" s="28" t="inlineStr">
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>70  Year</t>
         </is>
       </c>
-      <c r="H4" s="35" t="inlineStr">
+      <c r="H4" s="32" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6400,7 +6106,7 @@
           <t>Biospecimen retention contains DNA indicator</t>
         </is>
       </c>
-      <c r="G5" s="28" t="inlineStr">
+      <c r="G5" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6452,7 +6158,7 @@
           <t>Biospecimen retention indicator</t>
         </is>
       </c>
-      <c r="G6" s="28" t="inlineStr">
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6500,7 +6206,7 @@
         </is>
       </c>
       <c r="F7" s="14" t="n"/>
-      <c r="G7" s="28" t="inlineStr">
+      <c r="G7" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6656,7 +6362,7 @@
           <t>Minimum Response Duration</t>
         </is>
       </c>
-      <c r="G10" s="28" t="inlineStr">
+      <c r="G10" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '1 Day' , 'StudyIntervention_2': '1 Day'}</t>
         </is>
@@ -6713,7 +6419,7 @@
           <t>Background treatment</t>
         </is>
       </c>
-      <c r="G11" s="28" t="inlineStr">
+      <c r="G11" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6757,7 +6463,7 @@
           <t>Data Monitoring Committee Indicator</t>
         </is>
       </c>
-      <c r="G12" s="28" t="inlineStr">
+      <c r="G12" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6809,7 +6515,7 @@
           <t>Dosage Levels</t>
         </is>
       </c>
-      <c r="G13" s="28" t="inlineStr">
+      <c r="G13" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 3.0, 'StudyIntervention_2': 1.0}</t>
         </is>
@@ -6866,7 +6572,7 @@
           <t>Dose Form</t>
         </is>
       </c>
-      <c r="G14" s="28" t="inlineStr">
+      <c r="G14" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6918,7 +6624,7 @@
           <t>Administration Frequency</t>
         </is>
       </c>
-      <c r="G15" s="28" t="inlineStr">
+      <c r="G15" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'Once', 'StudyIntervention_2': 'Once'}</t>
         </is>
@@ -6928,17 +6634,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I15" s="28" t="inlineStr">
+      <c r="I15" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'C64576', 'StudyIntervention_2': 'C64576'}</t>
         </is>
       </c>
-      <c r="J15" s="28" t="inlineStr">
+      <c r="J15" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K15" s="28" t="inlineStr">
+      <c r="K15" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
@@ -6975,7 +6681,7 @@
           <t>Dosage Units</t>
         </is>
       </c>
-      <c r="G16" s="28" t="inlineStr">
+      <c r="G16" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'Milligram', 'StudyIntervention_2': 'Milligram'}</t>
         </is>
@@ -6985,17 +6691,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I16" s="28" t="inlineStr">
+      <c r="I16" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'C28253', 'StudyIntervention_2': 'C28253'}</t>
         </is>
       </c>
-      <c r="J16" s="28" t="inlineStr">
+      <c r="J16" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K16" s="28" t="inlineStr">
+      <c r="K16" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
@@ -7024,7 +6730,7 @@
           <t>Extension Trial Indicator</t>
         </is>
       </c>
-      <c r="G17" s="36" t="inlineStr">
+      <c r="G17" s="33" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7116,7 +6822,7 @@
           <t>Healthy Subject Indicator Study Population / Cohort</t>
         </is>
       </c>
-      <c r="G19" s="28" t="inlineStr">
+      <c r="G19" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7160,7 +6866,7 @@
           <t>Study design Diagnosis or Condition</t>
         </is>
       </c>
-      <c r="G20" s="28" t="inlineStr">
+      <c r="G20" s="25" t="inlineStr">
         <is>
           <t>{'Indication_1': 'T1DM' , 'Indication_2': 'T2DM'}</t>
         </is>
@@ -7209,7 +6915,7 @@
           <t>Intervention Model</t>
         </is>
       </c>
-      <c r="G21" s="29" t="inlineStr">
+      <c r="G21" s="26" t="inlineStr">
         <is>
           <t>Parallel Study</t>
         </is>
@@ -7219,17 +6925,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I21" s="29" t="inlineStr">
+      <c r="I21" s="26" t="inlineStr">
         <is>
           <t>C82639</t>
         </is>
       </c>
-      <c r="J21" s="29" t="inlineStr">
+      <c r="J21" s="26" t="inlineStr">
         <is>
           <t>//www.cdisc.org</t>
         </is>
       </c>
-      <c r="K21" s="29" t="inlineStr">
+      <c r="K21" s="26" t="inlineStr">
         <is>
           <t>2024-09-27</t>
         </is>
@@ -7266,7 +6972,7 @@
           <t>Intervention Type</t>
         </is>
       </c>
-      <c r="G22" s="28" t="inlineStr">
+      <c r="G22" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'Pharmacologic Substance', 'StudyIntervention_2': 'Pharmacologic Substance'}</t>
         </is>
@@ -7276,17 +6982,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I22" s="28" t="inlineStr">
+      <c r="I22" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'C1909', 'StudyIntervention_2': 'C1909'}</t>
         </is>
       </c>
-      <c r="J22" s="28" t="inlineStr">
+      <c r="J22" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K22" s="28" t="inlineStr">
+      <c r="K22" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
@@ -7315,7 +7021,7 @@
           <t>Trial Duration Value + Units</t>
         </is>
       </c>
-      <c r="G23" s="28" t="inlineStr">
+      <c r="G23" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7408,7 +7114,7 @@
           <t>Number of Arms</t>
         </is>
       </c>
-      <c r="G25" s="28" t="inlineStr">
+      <c r="G25" s="25" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -7457,7 +7163,7 @@
           <t>Number of Groups/Cohorts</t>
         </is>
       </c>
-      <c r="G26" s="29" t="inlineStr">
+      <c r="G26" s="26" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -7558,7 +7264,7 @@
           <t>Exploratory Objective</t>
         </is>
       </c>
-      <c r="G28" s="28" t="inlineStr">
+      <c r="G28" s="25" t="inlineStr">
         <is>
           <t>{'Objective_5': 'Explore the formation of anti-glucagon antibodies to glucagon' , 'Objective_6': 'To evaluate the recovery from clinical symptoms of hypoglycemia'}</t>
         </is>
@@ -7615,7 +7321,7 @@
           <t>Primary Objective</t>
         </is>
       </c>
-      <c r="G29" s="28" t="inlineStr">
+      <c r="G29" s="25" t="inlineStr">
         <is>
           <t>{'Objective_1': 'To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%'}</t>
         </is>
@@ -7672,7 +7378,7 @@
           <t>Secondary Objective</t>
         </is>
       </c>
-      <c r="G30" s="28" t="inlineStr">
+      <c r="G30" s="25" t="inlineStr">
         <is>
           <t>{'Objective_2': 'To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG' , 'Objective_3': 'To characterize the PK profile of 3 mg LY900018\ncompared to 1 mg IMG' , 'Objective_4': 'To characterize the PD profile of 3 mg LY900018\ncompared to 1 mg IMG'}</t>
         </is>
@@ -7721,22 +7427,22 @@
           <t>Observational Model</t>
         </is>
       </c>
-      <c r="G31" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I31" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J31" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K31" s="31" t="inlineStr">
+      <c r="G31" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I31" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J31" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K31" s="28" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7765,22 +7471,22 @@
           <t>Observational Time Perspective</t>
         </is>
       </c>
-      <c r="G32" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I32" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J32" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K32" s="29" t="inlineStr">
+      <c r="G32" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I32" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J32" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K32" s="26" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7809,7 +7515,7 @@
           <t>Observational Study Population Description</t>
         </is>
       </c>
-      <c r="G33" s="29" t="inlineStr">
+      <c r="G33" s="26" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7853,22 +7559,22 @@
           <t>Observational Study Sampling Method</t>
         </is>
       </c>
-      <c r="G34" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I34" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J34" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K34" s="29" t="inlineStr">
+      <c r="G34" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I34" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J34" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K34" s="26" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -7905,7 +7611,7 @@
           <t>Exploratory Outcome Measure</t>
         </is>
       </c>
-      <c r="G35" s="28" t="inlineStr">
+      <c r="G35" s="25" t="inlineStr">
         <is>
           <t>{ , }</t>
         </is>
@@ -7962,7 +7668,7 @@
           <t>Primary Outcome Measure</t>
         </is>
       </c>
-      <c r="G36" s="28" t="inlineStr">
+      <c r="G36" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8014,7 +7720,7 @@
           <t>Secondary Outcome Measure</t>
         </is>
       </c>
-      <c r="G37" s="28" t="inlineStr">
+      <c r="G37" s="25" t="inlineStr">
         <is>
           <t>{ ,  , }</t>
         </is>
@@ -8067,7 +7773,7 @@
           <t>Pharmacologic Class</t>
         </is>
       </c>
-      <c r="G38" s="28" t="inlineStr">
+      <c r="G38" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8111,7 +7817,7 @@
           <t>Pediatric Investigation Plan Indicator</t>
         </is>
       </c>
-      <c r="G39" s="28" t="inlineStr">
+      <c r="G39" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8155,7 +7861,7 @@
           <t>Target Enrollment Number</t>
         </is>
       </c>
-      <c r="G40" s="28" t="inlineStr">
+      <c r="G40" s="25" t="inlineStr">
         <is>
           <t>75.0</t>
         </is>
@@ -8208,7 +7914,7 @@
           <t>Planned Duration of Intervention Value + Unit</t>
         </is>
       </c>
-      <c r="G41" s="29" t="inlineStr">
+      <c r="G41" s="26" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
         </is>
@@ -8257,7 +7963,7 @@
           <t>Randomized Indicator</t>
         </is>
       </c>
-      <c r="G42" s="28" t="inlineStr">
+      <c r="G42" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8301,7 +8007,7 @@
           <t>Rare disease indicator</t>
         </is>
       </c>
-      <c r="G43" s="29" t="inlineStr">
+      <c r="G43" s="26" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8405,7 +8111,7 @@
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="G45" s="28" t="inlineStr">
+      <c r="G45" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
         </is>
@@ -8415,17 +8121,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I45" s="28" t="inlineStr">
+      <c r="I45" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'C38284', 'StudyIntervention_2': 'C28161'}</t>
         </is>
       </c>
-      <c r="J45" s="28" t="inlineStr">
+      <c r="J45" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K45" s="28" t="inlineStr">
+      <c r="K45" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
@@ -8550,7 +8256,7 @@
           <t>Sponsor Name - Organization</t>
         </is>
       </c>
-      <c r="G48" s="28" t="inlineStr">
+      <c r="G48" s="25" t="inlineStr">
         <is>
           <t>Eli Lilly Japan K.K</t>
         </is>
@@ -8691,7 +8397,7 @@
           <t>Study Type</t>
         </is>
       </c>
-      <c r="G51" s="31" t="inlineStr">
+      <c r="G51" s="28" t="inlineStr">
         <is>
           <t>Interventional Study</t>
         </is>
@@ -8701,17 +8407,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I51" s="31" t="inlineStr">
+      <c r="I51" s="28" t="inlineStr">
         <is>
           <t>C98388</t>
         </is>
       </c>
-      <c r="J51" s="31" t="inlineStr">
+      <c r="J51" s="28" t="inlineStr">
         <is>
           <t>//www.cdisc.org</t>
         </is>
       </c>
-      <c r="K51" s="31" t="inlineStr">
+      <c r="K51" s="28" t="inlineStr">
         <is>
           <t>2024-09-27</t>
         </is>
@@ -8740,7 +8446,7 @@
           <t>Blinding Schema</t>
         </is>
       </c>
-      <c r="G52" s="28" t="inlineStr">
+      <c r="G52" s="25" t="inlineStr">
         <is>
           <t>Open Label Study</t>
         </is>
@@ -8750,17 +8456,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I52" s="28" t="inlineStr">
+      <c r="I52" s="25" t="inlineStr">
         <is>
           <t>C49659</t>
         </is>
       </c>
-      <c r="J52" s="28" t="inlineStr">
+      <c r="J52" s="25" t="inlineStr">
         <is>
           <t>//www.cdisc.org</t>
         </is>
       </c>
-      <c r="K52" s="28" t="inlineStr">
+      <c r="K52" s="25" t="inlineStr">
         <is>
           <t>2024-09-27</t>
         </is>
@@ -8789,22 +8495,22 @@
           <t>Intervention Control Type</t>
         </is>
       </c>
-      <c r="G53" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I53" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J53" s="29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K53" s="29" t="inlineStr">
+      <c r="G53" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I53" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J53" s="26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K53" s="26" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8833,22 +8539,22 @@
           <t>Therapeutic Area</t>
         </is>
       </c>
-      <c r="G54" s="28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I54" s="28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J54" s="28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K54" s="28" t="inlineStr">
+      <c r="G54" s="25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I54" s="25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J54" s="25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K54" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8881,7 +8587,7 @@
           <t>Trial Intent Types</t>
         </is>
       </c>
-      <c r="G55" s="28" t="inlineStr">
+      <c r="G55" s="25" t="inlineStr">
         <is>
           <t>{'Code_129': 'Basic Research' , 'Code_130': 'Device Feasibility Study'}</t>
         </is>
@@ -8891,17 +8597,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I55" s="28" t="inlineStr">
+      <c r="I55" s="25" t="inlineStr">
         <is>
           <t>{'Code_129': 'C15714' , 'Code_130': 'C139174'}</t>
         </is>
       </c>
-      <c r="J55" s="28" t="inlineStr">
+      <c r="J55" s="25" t="inlineStr">
         <is>
           <t>{'Code_129': 'http://www.cdisc.org' , 'Code_130': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K55" s="28" t="inlineStr">
+      <c r="K55" s="25" t="inlineStr">
         <is>
           <t>{'Code_129': '2024-09-27' , 'Code_130': '2024-09-27'}</t>
         </is>
@@ -8930,7 +8636,7 @@
           <t>Full Title</t>
         </is>
       </c>
-      <c r="G56" s="28" t="inlineStr">
+      <c r="G56" s="25" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -8974,27 +8680,27 @@
           <t>Trial Phase</t>
         </is>
       </c>
-      <c r="G57" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H57" s="35" t="inlineStr">
+      <c r="G57" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H57" s="32" t="inlineStr">
         <is>
           <t>NI</t>
         </is>
       </c>
-      <c r="I57" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J57" s="31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K57" s="31" t="inlineStr">
+      <c r="I57" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J57" s="28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K57" s="28" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -9031,12 +8737,12 @@
           <t>Investigational Intervention</t>
         </is>
       </c>
-      <c r="G58" s="28" t="inlineStr">
+      <c r="G58" s="25" t="inlineStr">
         <is>
           <t>{'StudyIntervention_1': 'LY900018' , 'StudyIntervention_2': 'GlucaGen'}</t>
         </is>
       </c>
-      <c r="H58" s="35" t="inlineStr">
+      <c r="H58" s="32" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -9080,7 +8786,7 @@
           <t>Trial Type</t>
         </is>
       </c>
-      <c r="G59" s="28" t="inlineStr">
+      <c r="G59" s="25" t="inlineStr">
         <is>
           <t>{'Code_131': 'Efficacy Study'}</t>
         </is>
@@ -9090,17 +8796,17 @@
           <t> </t>
         </is>
       </c>
-      <c r="I59" s="28" t="inlineStr">
+      <c r="I59" s="25" t="inlineStr">
         <is>
           <t>{'Code_131': 'C49666'}</t>
         </is>
       </c>
-      <c r="J59" s="28" t="inlineStr">
+      <c r="J59" s="25" t="inlineStr">
         <is>
           <t>{'Code_131': 'http://www.cdisc.org'}</t>
         </is>
       </c>
-      <c r="K59" s="28" t="inlineStr">
+      <c r="K59" s="25" t="inlineStr">
         <is>
           <t>{'Code_131': '2024-09-27'}</t>
         </is>

</xml_diff>